<commit_message>
last modifying before testing
-generate new images
-adjust script with random 3rd feature
-add list to table
</commit_message>
<xml_diff>
--- a/stimuli_transparent.xlsx
+++ b/stimuli_transparent.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SFB833-FS\Documents\GitHub\huashan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hening Wang\Documents\GitHub\huashan\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6A68C44-06E2-4A42-B2DF-7134C6CC680A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -486,7 +499,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -670,7 +683,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0"/>
@@ -1827,30 +1840,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB160"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15.4" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="15.4" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" style="1" customWidth="1"/>
-    <col min="9" max="16" width="8.7109375" style="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" style="1" customWidth="1"/>
-    <col min="18" max="22" width="8.7109375" style="1" customWidth="1"/>
-    <col min="23" max="23" width="18.28515625" style="1" customWidth="1"/>
-    <col min="24" max="24" width="53.28515625" style="1" customWidth="1"/>
-    <col min="25" max="27" width="55.28515625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="26.28515625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="8.85546875" style="1" customWidth="1"/>
-    <col min="30" max="16384" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="8.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.26953125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.1796875" style="1" customWidth="1"/>
+    <col min="9" max="16" width="8.7265625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="12.453125" style="1" customWidth="1"/>
+    <col min="18" max="22" width="8.7265625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="18.26953125" style="1" customWidth="1"/>
+    <col min="24" max="24" width="53.26953125" style="1" customWidth="1"/>
+    <col min="25" max="27" width="55.26953125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="26.26953125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="8.81640625" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="13.5" customHeight="1">
@@ -1955,15 +1970,15 @@
       </c>
       <c r="E2" s="7">
         <f t="shared" ref="E2:I51" ca="1" si="1">RANDBETWEEN(9,10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="8">
         <f t="shared" ref="F2:J51" ca="1" si="2">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G2" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -1975,7 +1990,7 @@
       </c>
       <c r="J2" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>28</v>
@@ -2046,27 +2061,27 @@
       </c>
       <c r="E3" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G3" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I3" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K3" s="4" t="s">
         <v>30</v>
@@ -2222,15 +2237,15 @@
       </c>
       <c r="E5" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G5" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -2242,7 +2257,7 @@
       </c>
       <c r="J5" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>29</v>
@@ -2313,11 +2328,11 @@
       </c>
       <c r="E6" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G6" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -2329,7 +2344,7 @@
       </c>
       <c r="I6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -2489,7 +2504,7 @@
       </c>
       <c r="E8" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F8" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -2497,19 +2512,19 @@
       </c>
       <c r="G8" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H8" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J8" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>28</v>
@@ -2588,15 +2603,15 @@
       </c>
       <c r="G9" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I9" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J9" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -2756,23 +2771,23 @@
       </c>
       <c r="E11" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F11" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I11" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -2859,15 +2874,15 @@
       </c>
       <c r="H12" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I12" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J12" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>30</v>
@@ -3023,7 +3038,7 @@
       </c>
       <c r="E14" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F14" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -3031,7 +3046,7 @@
       </c>
       <c r="G14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H14" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -3039,7 +3054,7 @@
       </c>
       <c r="I14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J14" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -3122,7 +3137,7 @@
       </c>
       <c r="G15" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H15" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -3134,7 +3149,7 @@
       </c>
       <c r="J15" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>30</v>
@@ -3290,7 +3305,7 @@
       </c>
       <c r="E17" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F17" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -3306,11 +3321,11 @@
       </c>
       <c r="I17" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J17" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>28</v>
@@ -3381,23 +3396,23 @@
       </c>
       <c r="E18" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F18" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H18" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J18" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -3573,11 +3588,11 @@
       </c>
       <c r="I20" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>28</v>
@@ -3652,7 +3667,7 @@
       </c>
       <c r="F21" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G21" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -3660,15 +3675,15 @@
       </c>
       <c r="H21" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I21" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>30</v>
@@ -3828,15 +3843,15 @@
       </c>
       <c r="F23" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G23" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H23" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I23" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -3844,7 +3859,7 @@
       </c>
       <c r="J23" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K23" s="4" t="s">
         <v>64</v>
@@ -3915,7 +3930,7 @@
       </c>
       <c r="E24" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -3931,11 +3946,11 @@
       </c>
       <c r="I24" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J24" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K24" s="4" t="s">
         <v>30</v>
@@ -4099,11 +4114,11 @@
       </c>
       <c r="G26" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H26" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I26" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -4182,7 +4197,7 @@
       </c>
       <c r="E27" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F27" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -4198,7 +4213,7 @@
       </c>
       <c r="I27" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J27" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -4358,15 +4373,15 @@
       </c>
       <c r="E29" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F29" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H29" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -4453,7 +4468,7 @@
       </c>
       <c r="F30" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G30" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -4461,11 +4476,11 @@
       </c>
       <c r="H30" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I30" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J30" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -4625,7 +4640,7 @@
       </c>
       <c r="E32" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F32" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -4637,7 +4652,7 @@
       </c>
       <c r="H32" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I32" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -4645,7 +4660,7 @@
       </c>
       <c r="J32" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>74</v>
@@ -4716,15 +4731,15 @@
       </c>
       <c r="E33" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F33" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G33" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H33" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -4732,7 +4747,7 @@
       </c>
       <c r="I33" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J33" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -4896,7 +4911,7 @@
       </c>
       <c r="F35" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G35" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -4904,11 +4919,11 @@
       </c>
       <c r="H35" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I35" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J35" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -4983,11 +4998,11 @@
       </c>
       <c r="E36" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F36" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G36" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -4995,7 +5010,7 @@
       </c>
       <c r="H36" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -5003,7 +5018,7 @@
       </c>
       <c r="J36" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K36" s="4" t="s">
         <v>30</v>
@@ -5163,7 +5178,7 @@
       </c>
       <c r="F38" s="8">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G38" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -5171,7 +5186,7 @@
       </c>
       <c r="H38" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I38" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -5179,7 +5194,7 @@
       </c>
       <c r="J38" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>84</v>
@@ -5262,7 +5277,7 @@
       </c>
       <c r="H39" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I39" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -5430,23 +5445,23 @@
       </c>
       <c r="F41" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G41" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H41" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I41" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J41" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>84</v>
@@ -5521,7 +5536,7 @@
       </c>
       <c r="F42" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G42" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -5529,7 +5544,7 @@
       </c>
       <c r="H42" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I42" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -5537,7 +5552,7 @@
       </c>
       <c r="J42" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>30</v>
@@ -5705,7 +5720,7 @@
       </c>
       <c r="H44" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I44" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -5784,15 +5799,15 @@
       </c>
       <c r="E45" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F45" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G45" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H45" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -5800,7 +5815,7 @@
       </c>
       <c r="I45" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J45" s="9">
         <f t="shared" ca="1" si="2"/>
@@ -5960,7 +5975,7 @@
       </c>
       <c r="E47" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F47" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -5968,19 +5983,19 @@
       </c>
       <c r="G47" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H47" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I47" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J47" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>94</v>
@@ -6051,7 +6066,7 @@
       </c>
       <c r="E48" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F48" s="8">
         <f t="shared" ca="1" si="2"/>
@@ -6059,7 +6074,7 @@
       </c>
       <c r="G48" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H48" s="6">
         <f t="shared" ca="1" si="2"/>
@@ -6067,11 +6082,11 @@
       </c>
       <c r="I48" s="6">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J48" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K48" s="4" t="s">
         <v>30</v>
@@ -6227,7 +6242,7 @@
       </c>
       <c r="E50" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F50" s="8">
         <f t="shared" ca="1" si="1"/>
@@ -6235,19 +6250,19 @@
       </c>
       <c r="G50" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H50" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I50" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J50" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K50" s="4" t="s">
         <v>53</v>
@@ -6318,11 +6333,11 @@
       </c>
       <c r="E51" s="7">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F51" s="8">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G51" s="6">
         <f t="shared" ca="1" si="1"/>
@@ -6334,11 +6349,11 @@
       </c>
       <c r="I51" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J51" s="9">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>30</v>
@@ -6494,15 +6509,15 @@
       </c>
       <c r="E53" s="7">
         <f t="shared" ref="E53:I102" ca="1" si="4">RANDBETWEEN(9,10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F53" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G53" s="6">
         <f t="shared" ref="G53:J114" ca="1" si="5">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H53" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -6510,11 +6525,11 @@
       </c>
       <c r="I53" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J53" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K53" s="4" t="s">
         <v>29</v>
@@ -6593,7 +6608,7 @@
       </c>
       <c r="G54" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H54" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -6605,7 +6620,7 @@
       </c>
       <c r="J54" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K54" s="4" t="s">
         <v>30</v>
@@ -6761,15 +6776,15 @@
       </c>
       <c r="E56" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F56" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G56" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H56" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -6777,11 +6792,11 @@
       </c>
       <c r="I56" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J56" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K56" s="4" t="s">
         <v>29</v>
@@ -6852,11 +6867,11 @@
       </c>
       <c r="E57" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F57" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G57" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -6868,11 +6883,11 @@
       </c>
       <c r="I57" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J57" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K57" s="4" t="s">
         <v>30</v>
@@ -7028,11 +7043,11 @@
       </c>
       <c r="E59" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F59" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G59" s="6">
         <f t="shared" ca="1" si="4"/>
@@ -7048,7 +7063,7 @@
       </c>
       <c r="J59" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K59" s="4" t="s">
         <v>64</v>
@@ -7119,7 +7134,7 @@
       </c>
       <c r="E60" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F60" s="8">
         <f t="shared" ca="1" si="4"/>
@@ -7139,7 +7154,7 @@
       </c>
       <c r="J60" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K60" s="4" t="s">
         <v>30</v>
@@ -7299,15 +7314,15 @@
       </c>
       <c r="F62" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G62" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H62" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I62" s="6">
         <f t="shared" ca="1" si="4"/>
@@ -7315,7 +7330,7 @@
       </c>
       <c r="J62" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K62" s="4" t="s">
         <v>29</v>
@@ -7390,11 +7405,11 @@
       </c>
       <c r="F63" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G63" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H63" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -7402,11 +7417,11 @@
       </c>
       <c r="I63" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J63" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K63" s="4" t="s">
         <v>30</v>
@@ -7562,23 +7577,23 @@
       </c>
       <c r="E65" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F65" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G65" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H65" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I65" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J65" s="9">
         <f t="shared" ca="1" si="5"/>
@@ -7642,7 +7657,7 @@
         <v>8</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f t="shared" ref="B66:B97" si="6">C66&amp;""&amp;D66</f>
+        <f t="shared" ref="B66:B82" si="6">C66&amp;""&amp;D66</f>
         <v>erdf</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -7653,19 +7668,19 @@
       </c>
       <c r="E66" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F66" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G66" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H66" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I66" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -7829,7 +7844,7 @@
       </c>
       <c r="E68" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F68" s="8">
         <f t="shared" ca="1" si="4"/>
@@ -7849,7 +7864,7 @@
       </c>
       <c r="J68" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K68" s="4" t="s">
         <v>74</v>
@@ -7928,15 +7943,15 @@
       </c>
       <c r="G69" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H69" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I69" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J69" s="9">
         <f t="shared" ca="1" si="5"/>
@@ -8100,11 +8115,11 @@
       </c>
       <c r="F71" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G71" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H71" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -8112,11 +8127,11 @@
       </c>
       <c r="I71" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J71" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K71" s="4" t="s">
         <v>74</v>
@@ -8187,7 +8202,7 @@
       </c>
       <c r="E72" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F72" s="8">
         <f t="shared" ca="1" si="4"/>
@@ -8195,11 +8210,11 @@
       </c>
       <c r="G72" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H72" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I72" s="6">
         <f t="shared" ca="1" si="4"/>
@@ -8207,7 +8222,7 @@
       </c>
       <c r="J72" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K72" s="4" t="s">
         <v>30</v>
@@ -8367,15 +8382,15 @@
       </c>
       <c r="F74" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G74" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H74" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I74" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -8383,7 +8398,7 @@
       </c>
       <c r="J74" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K74" s="4" t="s">
         <v>29</v>
@@ -8458,19 +8473,19 @@
       </c>
       <c r="F75" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G75" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H75" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I75" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J75" s="9">
         <f t="shared" ca="1" si="5"/>
@@ -8646,11 +8661,11 @@
       </c>
       <c r="I77" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J77" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K77" s="4" t="s">
         <v>84</v>
@@ -8725,7 +8740,7 @@
       </c>
       <c r="F78" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G78" s="6">
         <f t="shared" ca="1" si="4"/>
@@ -8737,7 +8752,7 @@
       </c>
       <c r="I78" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J78" s="9">
         <f t="shared" ca="1" si="5"/>
@@ -8905,7 +8920,7 @@
       </c>
       <c r="G80" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H80" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -8917,7 +8932,7 @@
       </c>
       <c r="J80" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K80" s="4" t="s">
         <v>29</v>
@@ -8996,11 +9011,11 @@
       </c>
       <c r="G81" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H81" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I81" s="6">
         <f t="shared" ca="1" si="4"/>
@@ -9168,7 +9183,7 @@
       </c>
       <c r="F83" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G83" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -9176,7 +9191,7 @@
       </c>
       <c r="H83" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I83" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -9257,27 +9272,27 @@
       </c>
       <c r="E84" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F84" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G84" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H84" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I84" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J84" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K84" s="4" t="s">
         <v>30</v>
@@ -9453,7 +9468,7 @@
       </c>
       <c r="I86" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J86" s="9">
         <f t="shared" ca="1" si="5"/>
@@ -9530,7 +9545,7 @@
       </c>
       <c r="E87" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F87" s="8">
         <f t="shared" ca="1" si="4"/>
@@ -9542,7 +9557,7 @@
       </c>
       <c r="H87" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I87" s="6">
         <f t="shared" ca="1" si="4"/>
@@ -9550,7 +9565,7 @@
       </c>
       <c r="J87" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K87" s="4" t="s">
         <v>30</v>
@@ -9710,7 +9725,7 @@
       </c>
       <c r="E89" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F89" s="8">
         <f t="shared" ca="1" si="4"/>
@@ -9722,15 +9737,15 @@
       </c>
       <c r="H89" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I89" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J89" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K89" s="4" t="s">
         <v>53</v>
@@ -9807,23 +9822,23 @@
       </c>
       <c r="F90" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G90" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H90" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I90" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J90" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K90" s="4" t="s">
         <v>30</v>
@@ -9983,15 +9998,15 @@
       </c>
       <c r="E92" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F92" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G92" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H92" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -10003,7 +10018,7 @@
       </c>
       <c r="J92" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K92" s="4" t="s">
         <v>53</v>
@@ -10088,11 +10103,11 @@
       </c>
       <c r="H93" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I93" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J93" s="9">
         <f t="shared" ca="1" si="5"/>
@@ -10272,11 +10287,11 @@
       </c>
       <c r="I95" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J95" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K95" s="4" t="s">
         <v>74</v>
@@ -10361,15 +10376,15 @@
       </c>
       <c r="H96" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I96" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J96" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K96" s="4" t="s">
         <v>30</v>
@@ -10533,7 +10548,7 @@
       </c>
       <c r="F98" s="8">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G98" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -10545,11 +10560,11 @@
       </c>
       <c r="I98" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J98" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K98" s="4" t="s">
         <v>53</v>
@@ -10622,7 +10637,7 @@
       </c>
       <c r="E99" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F99" s="8">
         <f t="shared" ca="1" si="4"/>
@@ -10630,15 +10645,15 @@
       </c>
       <c r="G99" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H99" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I99" s="6">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J99" s="9">
         <f t="shared" ca="1" si="5"/>
@@ -10802,7 +10817,7 @@
       </c>
       <c r="E101" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F101" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
@@ -10810,7 +10825,7 @@
       </c>
       <c r="G101" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H101" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -10818,11 +10833,11 @@
       </c>
       <c r="I101" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J101" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K101" s="4" t="s">
         <v>53</v>
@@ -10895,27 +10910,27 @@
       </c>
       <c r="E102" s="7">
         <f t="shared" ca="1" si="4"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F102" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G102" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H102" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I102" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J102" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K102" s="4" t="s">
         <v>30</v>
@@ -11075,7 +11090,7 @@
       </c>
       <c r="E104" s="7">
         <f t="shared" ref="E104:I154" ca="1" si="8">RANDBETWEEN(9,10)</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F104" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -11087,7 +11102,7 @@
       </c>
       <c r="H104" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I104" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -11095,7 +11110,7 @@
       </c>
       <c r="J104" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K104" s="4" t="s">
         <v>84</v>
@@ -11172,7 +11187,7 @@
       </c>
       <c r="F105" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G105" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -11184,11 +11199,11 @@
       </c>
       <c r="I105" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J105" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K105" s="4" t="s">
         <v>30</v>
@@ -11348,7 +11363,7 @@
       </c>
       <c r="E107" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F107" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -11360,11 +11375,11 @@
       </c>
       <c r="H107" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I107" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J107" s="9">
         <f t="shared" ca="1" si="5"/>
@@ -11449,19 +11464,19 @@
       </c>
       <c r="G108" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H108" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I108" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J108" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K108" s="4" t="s">
         <v>30</v>
@@ -11621,15 +11636,15 @@
       </c>
       <c r="E110" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F110" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G110" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H110" s="6">
         <f t="shared" ca="1" si="5"/>
@@ -11641,7 +11656,7 @@
       </c>
       <c r="J110" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K110" s="4" t="s">
         <v>64</v>
@@ -11718,23 +11733,23 @@
       </c>
       <c r="F111" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G111" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H111" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I111" s="6">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J111" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K111" s="4" t="s">
         <v>30</v>
@@ -11894,7 +11909,7 @@
       </c>
       <c r="E113" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F113" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -11906,15 +11921,15 @@
       </c>
       <c r="H113" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I113" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J113" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K113" s="4" t="s">
         <v>74</v>
@@ -12007,7 +12022,7 @@
       </c>
       <c r="J114" s="9">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K114" s="4" t="s">
         <v>30</v>
@@ -12171,11 +12186,11 @@
       </c>
       <c r="F116" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G116" s="6">
         <f t="shared" ref="G116:J159" ca="1" si="10">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H116" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -12183,11 +12198,11 @@
       </c>
       <c r="I116" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J116" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K116" s="4" t="s">
         <v>64</v>
@@ -12260,19 +12275,19 @@
       </c>
       <c r="E117" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F117" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G117" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H117" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I117" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -12280,7 +12295,7 @@
       </c>
       <c r="J117" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K117" s="4" t="s">
         <v>30</v>
@@ -12440,15 +12455,15 @@
       </c>
       <c r="E119" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F119" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G119" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H119" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -12456,11 +12471,11 @@
       </c>
       <c r="I119" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J119" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K119" s="4" t="s">
         <v>64</v>
@@ -12533,11 +12548,11 @@
       </c>
       <c r="E120" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F120" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G120" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -12545,7 +12560,7 @@
       </c>
       <c r="H120" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I120" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -12553,7 +12568,7 @@
       </c>
       <c r="J120" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K120" s="4" t="s">
         <v>30</v>
@@ -12713,7 +12728,7 @@
       </c>
       <c r="E122" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F122" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -12721,11 +12736,11 @@
       </c>
       <c r="G122" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H122" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I122" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -12733,7 +12748,7 @@
       </c>
       <c r="J122" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K122" s="4" t="s">
         <v>84</v>
@@ -12810,7 +12825,7 @@
       </c>
       <c r="F123" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G123" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -12818,15 +12833,15 @@
       </c>
       <c r="H123" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I123" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J123" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K123" s="4" t="s">
         <v>30</v>
@@ -12990,23 +13005,23 @@
       </c>
       <c r="F125" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G125" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H125" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I125" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J125" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K125" s="4" t="s">
         <v>64</v>
@@ -13079,11 +13094,11 @@
       </c>
       <c r="E126" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F126" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G126" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -13095,11 +13110,11 @@
       </c>
       <c r="I126" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J126" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K126" s="4" t="s">
         <v>30</v>
@@ -13263,11 +13278,11 @@
       </c>
       <c r="F128" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G128" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H128" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -13275,7 +13290,7 @@
       </c>
       <c r="I128" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J128" s="9">
         <f t="shared" ca="1" si="10"/>
@@ -13352,7 +13367,7 @@
       </c>
       <c r="E129" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F129" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
@@ -13360,11 +13375,11 @@
       </c>
       <c r="G129" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H129" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I129" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -13372,7 +13387,7 @@
       </c>
       <c r="J129" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K129" s="4" t="s">
         <v>30</v>
@@ -13532,7 +13547,7 @@
       </c>
       <c r="E131" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F131" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -13544,15 +13559,15 @@
       </c>
       <c r="H131" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I131" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J131" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K131" s="4" t="s">
         <v>84</v>
@@ -13629,7 +13644,7 @@
       </c>
       <c r="F132" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G132" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -13805,7 +13820,7 @@
       </c>
       <c r="E134" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F134" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -13817,7 +13832,7 @@
       </c>
       <c r="H134" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I134" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -13825,7 +13840,7 @@
       </c>
       <c r="J134" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K134" s="4" t="s">
         <v>74</v>
@@ -13898,7 +13913,7 @@
       </c>
       <c r="E135" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F135" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -14078,19 +14093,19 @@
       </c>
       <c r="E137" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F137" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G137" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H137" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I137" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -14270,15 +14285,15 @@
       </c>
       <c r="H139" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I139" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J139" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K139" s="4" t="s">
         <v>28</v>
@@ -14351,7 +14366,7 @@
       </c>
       <c r="E140" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F140" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -14363,7 +14378,7 @@
       </c>
       <c r="H140" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I140" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -14371,7 +14386,7 @@
       </c>
       <c r="J140" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K140" s="4" t="s">
         <v>30</v>
@@ -14535,23 +14550,23 @@
       </c>
       <c r="F142" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G142" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H142" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I142" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J142" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K142" s="4" t="s">
         <v>74</v>
@@ -14624,7 +14639,7 @@
       </c>
       <c r="E143" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F143" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -14644,7 +14659,7 @@
       </c>
       <c r="J143" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="K143" s="4" t="s">
         <v>30</v>
@@ -14808,7 +14823,7 @@
       </c>
       <c r="F145" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G145" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -14816,15 +14831,15 @@
       </c>
       <c r="H145" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I145" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J145" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K145" s="4" t="s">
         <v>29</v>
@@ -14897,7 +14912,7 @@
       </c>
       <c r="E146" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F146" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -14909,7 +14924,7 @@
       </c>
       <c r="H146" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I146" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -14979,7 +14994,7 @@
         <v>175</v>
       </c>
       <c r="B147" s="2" t="str">
-        <f t="shared" ref="B147:B178" si="11">"f"&amp;C147&amp;""&amp;D147&amp;""&amp;Z147</f>
+        <f t="shared" ref="B147:B157" si="11">"f"&amp;C147&amp;""&amp;D147&amp;""&amp;Z147</f>
         <v>fbrcfs</v>
       </c>
       <c r="C147" s="2" t="s">
@@ -15081,11 +15096,11 @@
       </c>
       <c r="F148" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G148" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H148" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -15093,7 +15108,7 @@
       </c>
       <c r="I148" s="6">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="J148" s="9">
         <f t="shared" ca="1" si="10"/>
@@ -15174,15 +15189,15 @@
       </c>
       <c r="F149" s="8">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G149" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H149" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I149" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -15350,7 +15365,7 @@
       </c>
       <c r="E151" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F151" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -15358,7 +15373,7 @@
       </c>
       <c r="G151" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H151" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -15443,7 +15458,7 @@
       </c>
       <c r="E152" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F152" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -15451,11 +15466,11 @@
       </c>
       <c r="G152" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H152" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I152" s="6">
         <f t="shared" ca="1" si="8"/>
@@ -15463,7 +15478,7 @@
       </c>
       <c r="J152" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K152" s="4" t="s">
         <v>30</v>
@@ -15623,7 +15638,7 @@
       </c>
       <c r="E154" s="7">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F154" s="8">
         <f t="shared" ca="1" si="8"/>
@@ -15631,7 +15646,7 @@
       </c>
       <c r="G154" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H154" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -15643,7 +15658,7 @@
       </c>
       <c r="J154" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K154" s="4" t="s">
         <v>64</v>
@@ -15716,19 +15731,19 @@
       </c>
       <c r="E155" s="7">
         <f t="shared" ref="E155:I159" ca="1" si="12">RANDBETWEEN(9,10)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F155" s="8">
         <f t="shared" ca="1" si="12"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G155" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H155" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I155" s="6">
         <f t="shared" ca="1" si="12"/>
@@ -15736,7 +15751,7 @@
       </c>
       <c r="J155" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K155" s="4" t="s">
         <v>30</v>
@@ -15896,7 +15911,7 @@
       </c>
       <c r="E157" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F157" s="8">
         <f t="shared" ca="1" si="12"/>
@@ -15904,7 +15919,7 @@
       </c>
       <c r="G157" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H157" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -15912,11 +15927,11 @@
       </c>
       <c r="I157" s="6">
         <f t="shared" ca="1" si="12"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J157" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K157" s="4" t="s">
         <v>84</v>
@@ -15989,15 +16004,15 @@
       </c>
       <c r="E158" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F158" s="8">
         <f ca="1">RANDBETWEEN(1,3)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G158" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H158" s="6">
         <f t="shared" ca="1" si="10"/>
@@ -16005,7 +16020,7 @@
       </c>
       <c r="I158" s="6">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J158" s="9">
         <f t="shared" ca="1" si="10"/>
@@ -16080,7 +16095,7 @@
       </c>
       <c r="E159" s="7">
         <f t="shared" ca="1" si="12"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F159" s="8">
         <f t="shared" ca="1" si="12"/>
@@ -16100,7 +16115,7 @@
       </c>
       <c r="J159" s="9">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K159" s="4" t="s">
         <v>30</v>

</xml_diff>